<commit_message>
data exploration on time series
</commit_message>
<xml_diff>
--- a/Data/all_in_one_Time_sieries_data_color.xlsx
+++ b/Data/all_in_one_Time_sieries_data_color.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\linda\Documents\UNI\GitHub\ADS_year3_project_8\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{065D4A6F-528D-471E-941B-72F2299B7EED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8A7B4C-CBA1-4EE2-992A-CE693FE0A196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="42">
   <si>
     <t>Size_of_waiting_list</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -202,6 +202,15 @@
   </si>
   <si>
     <t>1998 - Q2</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>quarter</t>
   </si>
 </sst>
 </file>
@@ -1053,6 +1062,12 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="44" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1088,12 +1103,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="174" fontId="4" fillId="5" borderId="0" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="58" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1624,7 +1633,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AN36"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
@@ -2863,102 +2872,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="51" t="s">
+      <c r="A1" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="52" t="s">
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="52"/>
-      <c r="G1" s="52"/>
-      <c r="H1" s="52"/>
-      <c r="I1" s="52"/>
-      <c r="J1" s="52"/>
-      <c r="K1" s="52"/>
-      <c r="L1" s="53" t="s">
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
     </row>
     <row r="2" spans="1:16" ht="55.5" customHeight="1">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="50" t="s">
+      <c r="B2" s="58"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="53" t="s">
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="55" t="s">
         <v>28</v>
       </c>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
     </row>
     <row r="3" spans="1:16" ht="104" customHeight="1">
-      <c r="A3" s="54"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55" t="s">
+      <c r="A3" s="56"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="59"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61" t="s">
+      <c r="E3" s="61"/>
+      <c r="F3" s="62"/>
+      <c r="G3" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="63" t="s">
+      <c r="H3" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="63" t="s">
+      <c r="I3" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="L3" s="58" t="s">
+      <c r="L3" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="M3" s="57" t="s">
+      <c r="M3" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="N3" s="57" t="s">
+      <c r="N3" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="P3" s="57" t="s">
+      <c r="P3" s="59" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:16">
-      <c r="A4" s="54"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="64"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
+      <c r="A4" s="56"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57"/>
+      <c r="E4" s="61"/>
+      <c r="F4" s="62"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="L4" s="60"/>
+      <c r="M4" s="59"/>
+      <c r="N4" s="59"/>
+      <c r="O4" s="59"/>
+      <c r="P4" s="59"/>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="27">
@@ -7271,11 +7280,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="H3:H4"/>
-    <mergeCell ref="I3:I4"/>
-    <mergeCell ref="E2:K2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:K1"/>
     <mergeCell ref="L1:P1"/>
     <mergeCell ref="A3:C4"/>
     <mergeCell ref="D3:D4"/>
@@ -7289,6 +7293,11 @@
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="E2:K2"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:K1"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7300,7 +7309,7 @@
   <dimension ref="A1:F96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -7309,6 +7318,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
       <c r="D1" t="s">
         <v>34</v>
       </c>
@@ -7367,7 +7385,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="27" t="str">
-        <f>_xlfn.CONCAT(A4,B4)</f>
+        <f t="shared" ref="C4:C35" si="0">_xlfn.CONCAT(A4,B4)</f>
         <v>1998Q3</v>
       </c>
       <c r="D4" s="29">
@@ -7388,7 +7406,7 @@
         <v>14</v>
       </c>
       <c r="C5" s="27" t="str">
-        <f>_xlfn.CONCAT(A5,B5)</f>
+        <f t="shared" si="0"/>
         <v>1998Q4</v>
       </c>
       <c r="D5" s="29">
@@ -7409,7 +7427,7 @@
         <v>15</v>
       </c>
       <c r="C6" s="27" t="str">
-        <f>_xlfn.CONCAT(A6,B6)</f>
+        <f t="shared" si="0"/>
         <v>1999Q1</v>
       </c>
       <c r="D6" s="29">
@@ -7430,7 +7448,7 @@
         <v>12</v>
       </c>
       <c r="C7" s="27" t="str">
-        <f>_xlfn.CONCAT(A7,B7)</f>
+        <f t="shared" si="0"/>
         <v>1999Q2</v>
       </c>
       <c r="D7" s="29">
@@ -7451,7 +7469,7 @@
         <v>13</v>
       </c>
       <c r="C8" s="27" t="str">
-        <f>_xlfn.CONCAT(A8,B8)</f>
+        <f t="shared" si="0"/>
         <v>1999Q3</v>
       </c>
       <c r="D8" s="29">
@@ -7472,7 +7490,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="27" t="str">
-        <f>_xlfn.CONCAT(A9,B9)</f>
+        <f t="shared" si="0"/>
         <v>1999Q4</v>
       </c>
       <c r="D9" s="29">
@@ -7493,7 +7511,7 @@
         <v>15</v>
       </c>
       <c r="C10" s="27" t="str">
-        <f>_xlfn.CONCAT(A10,B10)</f>
+        <f t="shared" si="0"/>
         <v>2000Q1</v>
       </c>
       <c r="D10" s="29">
@@ -7514,7 +7532,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="27" t="str">
-        <f>_xlfn.CONCAT(A11,B11)</f>
+        <f t="shared" si="0"/>
         <v>2000Q2</v>
       </c>
       <c r="D11" s="29">
@@ -7535,7 +7553,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="27" t="str">
-        <f>_xlfn.CONCAT(A12,B12)</f>
+        <f t="shared" si="0"/>
         <v>2000Q3</v>
       </c>
       <c r="D12" s="29">
@@ -7556,7 +7574,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="27" t="str">
-        <f>_xlfn.CONCAT(A13,B13)</f>
+        <f t="shared" si="0"/>
         <v>2000Q4</v>
       </c>
       <c r="D13" s="29">
@@ -7577,7 +7595,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="27" t="str">
-        <f>_xlfn.CONCAT(A14,B14)</f>
+        <f t="shared" si="0"/>
         <v>2001Q1</v>
       </c>
       <c r="D14" s="29">
@@ -7598,7 +7616,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="27" t="str">
-        <f>_xlfn.CONCAT(A15,B15)</f>
+        <f t="shared" si="0"/>
         <v>2001Q2</v>
       </c>
       <c r="D15" s="29">
@@ -7619,7 +7637,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="27" t="str">
-        <f>_xlfn.CONCAT(A16,B16)</f>
+        <f t="shared" si="0"/>
         <v>2001Q3</v>
       </c>
       <c r="D16" s="29">
@@ -7640,7 +7658,7 @@
         <v>14</v>
       </c>
       <c r="C17" s="27" t="str">
-        <f>_xlfn.CONCAT(A17,B17)</f>
+        <f t="shared" si="0"/>
         <v>2001Q4</v>
       </c>
       <c r="D17" s="29">
@@ -7661,7 +7679,7 @@
         <v>15</v>
       </c>
       <c r="C18" s="27" t="str">
-        <f>_xlfn.CONCAT(A18,B18)</f>
+        <f t="shared" si="0"/>
         <v>2002Q1</v>
       </c>
       <c r="D18" s="29">
@@ -7682,7 +7700,7 @@
         <v>12</v>
       </c>
       <c r="C19" s="27" t="str">
-        <f>_xlfn.CONCAT(A19,B19)</f>
+        <f t="shared" si="0"/>
         <v>2002Q2</v>
       </c>
       <c r="D19" s="29">
@@ -7703,7 +7721,7 @@
         <v>13</v>
       </c>
       <c r="C20" s="27" t="str">
-        <f>_xlfn.CONCAT(A20,B20)</f>
+        <f t="shared" si="0"/>
         <v>2002Q3</v>
       </c>
       <c r="D20" s="29">
@@ -7724,7 +7742,7 @@
         <v>14</v>
       </c>
       <c r="C21" s="27" t="str">
-        <f>_xlfn.CONCAT(A21,B21)</f>
+        <f t="shared" si="0"/>
         <v>2002Q4</v>
       </c>
       <c r="D21" s="29">
@@ -7745,7 +7763,7 @@
         <v>15</v>
       </c>
       <c r="C22" s="27" t="str">
-        <f>_xlfn.CONCAT(A22,B22)</f>
+        <f t="shared" si="0"/>
         <v>2003Q1</v>
       </c>
       <c r="D22" s="29">
@@ -7766,7 +7784,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="27" t="str">
-        <f>_xlfn.CONCAT(A23,B23)</f>
+        <f t="shared" si="0"/>
         <v>2003Q2</v>
       </c>
       <c r="D23" s="29">
@@ -7787,7 +7805,7 @@
         <v>13</v>
       </c>
       <c r="C24" s="27" t="str">
-        <f>_xlfn.CONCAT(A24,B24)</f>
+        <f t="shared" si="0"/>
         <v>2003Q3</v>
       </c>
       <c r="D24" s="29">
@@ -7808,7 +7826,7 @@
         <v>14</v>
       </c>
       <c r="C25" s="27" t="str">
-        <f>_xlfn.CONCAT(A25,B25)</f>
+        <f t="shared" si="0"/>
         <v>2003Q4</v>
       </c>
       <c r="D25" s="29">
@@ -7829,7 +7847,7 @@
         <v>15</v>
       </c>
       <c r="C26" s="27" t="str">
-        <f>_xlfn.CONCAT(A26,B26)</f>
+        <f t="shared" si="0"/>
         <v>2004Q1</v>
       </c>
       <c r="D26" s="29">
@@ -7850,7 +7868,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="27" t="str">
-        <f>_xlfn.CONCAT(A27,B27)</f>
+        <f t="shared" si="0"/>
         <v>2004Q2</v>
       </c>
       <c r="D27" s="29">
@@ -7871,7 +7889,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="27" t="str">
-        <f>_xlfn.CONCAT(A28,B28)</f>
+        <f t="shared" si="0"/>
         <v>2004Q3</v>
       </c>
       <c r="D28" s="29">
@@ -7892,7 +7910,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="27" t="str">
-        <f>_xlfn.CONCAT(A29,B29)</f>
+        <f t="shared" si="0"/>
         <v>2004Q4</v>
       </c>
       <c r="D29" s="29">
@@ -7913,7 +7931,7 @@
         <v>15</v>
       </c>
       <c r="C30" s="27" t="str">
-        <f>_xlfn.CONCAT(A30,B30)</f>
+        <f t="shared" si="0"/>
         <v>2005Q1</v>
       </c>
       <c r="D30" s="29">
@@ -7934,7 +7952,7 @@
         <v>12</v>
       </c>
       <c r="C31" s="27" t="str">
-        <f>_xlfn.CONCAT(A31,B31)</f>
+        <f t="shared" si="0"/>
         <v>2005Q2</v>
       </c>
       <c r="D31" s="29">
@@ -7955,7 +7973,7 @@
         <v>13</v>
       </c>
       <c r="C32" s="27" t="str">
-        <f>_xlfn.CONCAT(A32,B32)</f>
+        <f t="shared" si="0"/>
         <v>2005Q3</v>
       </c>
       <c r="D32" s="29">
@@ -7976,7 +7994,7 @@
         <v>14</v>
       </c>
       <c r="C33" s="27" t="str">
-        <f>_xlfn.CONCAT(A33,B33)</f>
+        <f t="shared" si="0"/>
         <v>2005Q4</v>
       </c>
       <c r="D33" s="29">
@@ -7997,7 +8015,7 @@
         <v>15</v>
       </c>
       <c r="C34" s="27" t="str">
-        <f>_xlfn.CONCAT(A34,B34)</f>
+        <f t="shared" si="0"/>
         <v>2006Q1</v>
       </c>
       <c r="D34" s="29">
@@ -8018,7 +8036,7 @@
         <v>12</v>
       </c>
       <c r="C35" s="27" t="str">
-        <f>_xlfn.CONCAT(A35,B35)</f>
+        <f t="shared" si="0"/>
         <v>2006Q2</v>
       </c>
       <c r="D35" s="29">
@@ -8039,7 +8057,7 @@
         <v>13</v>
       </c>
       <c r="C36" s="27" t="str">
-        <f>_xlfn.CONCAT(A36,B36)</f>
+        <f t="shared" ref="C36:C67" si="1">_xlfn.CONCAT(A36,B36)</f>
         <v>2006Q3</v>
       </c>
       <c r="D36" s="29">
@@ -8060,7 +8078,7 @@
         <v>14</v>
       </c>
       <c r="C37" s="27" t="str">
-        <f>_xlfn.CONCAT(A37,B37)</f>
+        <f t="shared" si="1"/>
         <v>2006Q4</v>
       </c>
       <c r="D37" s="29">
@@ -8081,7 +8099,7 @@
         <v>15</v>
       </c>
       <c r="C38" s="27" t="str">
-        <f>_xlfn.CONCAT(A38,B38)</f>
+        <f t="shared" si="1"/>
         <v>2007Q1</v>
       </c>
       <c r="D38" s="29">
@@ -8102,7 +8120,7 @@
         <v>12</v>
       </c>
       <c r="C39" s="27" t="str">
-        <f>_xlfn.CONCAT(A39,B39)</f>
+        <f t="shared" si="1"/>
         <v>2007Q2</v>
       </c>
       <c r="D39" s="29">
@@ -8123,7 +8141,7 @@
         <v>13</v>
       </c>
       <c r="C40" s="27" t="str">
-        <f>_xlfn.CONCAT(A40,B40)</f>
+        <f t="shared" si="1"/>
         <v>2007Q3</v>
       </c>
       <c r="D40" s="29">
@@ -8144,7 +8162,7 @@
         <v>14</v>
       </c>
       <c r="C41" s="27" t="str">
-        <f>_xlfn.CONCAT(A41,B41)</f>
+        <f t="shared" si="1"/>
         <v>2007Q4</v>
       </c>
       <c r="D41" s="29">
@@ -8165,7 +8183,7 @@
         <v>15</v>
       </c>
       <c r="C42" s="27" t="str">
-        <f>_xlfn.CONCAT(A42,B42)</f>
+        <f t="shared" si="1"/>
         <v>2008Q1</v>
       </c>
       <c r="D42" s="29">
@@ -8186,7 +8204,7 @@
         <v>12</v>
       </c>
       <c r="C43" s="27" t="str">
-        <f>_xlfn.CONCAT(A43,B43)</f>
+        <f t="shared" si="1"/>
         <v>2008Q2</v>
       </c>
       <c r="D43" s="29">
@@ -8207,7 +8225,7 @@
         <v>13</v>
       </c>
       <c r="C44" s="27" t="str">
-        <f>_xlfn.CONCAT(A44,B44)</f>
+        <f t="shared" si="1"/>
         <v>2008Q3</v>
       </c>
       <c r="D44" s="29">
@@ -8228,7 +8246,7 @@
         <v>14</v>
       </c>
       <c r="C45" s="27" t="str">
-        <f>_xlfn.CONCAT(A45,B45)</f>
+        <f t="shared" si="1"/>
         <v>2008Q4</v>
       </c>
       <c r="D45" s="29">
@@ -8249,7 +8267,7 @@
         <v>15</v>
       </c>
       <c r="C46" s="27" t="str">
-        <f>_xlfn.CONCAT(A46,B46)</f>
+        <f t="shared" si="1"/>
         <v>2009Q1</v>
       </c>
       <c r="D46" s="29">
@@ -8270,7 +8288,7 @@
         <v>12</v>
       </c>
       <c r="C47" s="27" t="str">
-        <f>_xlfn.CONCAT(A47,B47)</f>
+        <f t="shared" si="1"/>
         <v>2009Q2</v>
       </c>
       <c r="D47" s="29">
@@ -8291,7 +8309,7 @@
         <v>13</v>
       </c>
       <c r="C48" s="27" t="str">
-        <f>_xlfn.CONCAT(A48,B48)</f>
+        <f t="shared" si="1"/>
         <v>2009Q3</v>
       </c>
       <c r="D48" s="29">
@@ -8312,7 +8330,7 @@
         <v>14</v>
       </c>
       <c r="C49" s="27" t="str">
-        <f>_xlfn.CONCAT(A49,B49)</f>
+        <f t="shared" si="1"/>
         <v>2009Q4</v>
       </c>
       <c r="D49" s="29">
@@ -8333,7 +8351,7 @@
         <v>15</v>
       </c>
       <c r="C50" s="27" t="str">
-        <f>_xlfn.CONCAT(A50,B50)</f>
+        <f t="shared" si="1"/>
         <v>2010Q1</v>
       </c>
       <c r="D50" s="29">
@@ -8354,7 +8372,7 @@
         <v>12</v>
       </c>
       <c r="C51" s="27" t="str">
-        <f>_xlfn.CONCAT(A51,B51)</f>
+        <f t="shared" si="1"/>
         <v>2010Q2</v>
       </c>
       <c r="D51" s="29">
@@ -8375,7 +8393,7 @@
         <v>13</v>
       </c>
       <c r="C52" s="27" t="str">
-        <f>_xlfn.CONCAT(A52,B52)</f>
+        <f t="shared" si="1"/>
         <v>2010Q3</v>
       </c>
       <c r="D52" s="29">
@@ -8396,7 +8414,7 @@
         <v>14</v>
       </c>
       <c r="C53" s="27" t="str">
-        <f>_xlfn.CONCAT(A53,B53)</f>
+        <f t="shared" si="1"/>
         <v>2010Q4</v>
       </c>
       <c r="D53" s="29">
@@ -8417,7 +8435,7 @@
         <v>15</v>
       </c>
       <c r="C54" s="27" t="str">
-        <f>_xlfn.CONCAT(A54,B54)</f>
+        <f t="shared" si="1"/>
         <v>2011Q1</v>
       </c>
       <c r="D54" s="29">
@@ -8438,7 +8456,7 @@
         <v>12</v>
       </c>
       <c r="C55" s="27" t="str">
-        <f>_xlfn.CONCAT(A55,B55)</f>
+        <f t="shared" si="1"/>
         <v>2011Q2</v>
       </c>
       <c r="D55" s="29">
@@ -8459,7 +8477,7 @@
         <v>13</v>
       </c>
       <c r="C56" s="27" t="str">
-        <f>_xlfn.CONCAT(A56,B56)</f>
+        <f t="shared" si="1"/>
         <v>2011Q3</v>
       </c>
       <c r="D56" s="29">
@@ -8480,7 +8498,7 @@
         <v>14</v>
       </c>
       <c r="C57" s="27" t="str">
-        <f>_xlfn.CONCAT(A57,B57)</f>
+        <f t="shared" si="1"/>
         <v>2011Q4</v>
       </c>
       <c r="D57" s="29">
@@ -8501,7 +8519,7 @@
         <v>15</v>
       </c>
       <c r="C58" s="27" t="str">
-        <f>_xlfn.CONCAT(A58,B58)</f>
+        <f t="shared" si="1"/>
         <v>2012Q1</v>
       </c>
       <c r="D58" s="29">
@@ -8522,7 +8540,7 @@
         <v>12</v>
       </c>
       <c r="C59" s="27" t="str">
-        <f>_xlfn.CONCAT(A59,B59)</f>
+        <f t="shared" si="1"/>
         <v>2012Q2</v>
       </c>
       <c r="D59" s="29">
@@ -8543,7 +8561,7 @@
         <v>13</v>
       </c>
       <c r="C60" s="27" t="str">
-        <f>_xlfn.CONCAT(A60,B60)</f>
+        <f t="shared" si="1"/>
         <v>2012Q3</v>
       </c>
       <c r="D60" s="29">
@@ -8564,7 +8582,7 @@
         <v>14</v>
       </c>
       <c r="C61" s="27" t="str">
-        <f>_xlfn.CONCAT(A61,B61)</f>
+        <f t="shared" si="1"/>
         <v>2012Q4</v>
       </c>
       <c r="D61" s="29">
@@ -8585,7 +8603,7 @@
         <v>15</v>
       </c>
       <c r="C62" s="27" t="str">
-        <f>_xlfn.CONCAT(A62,B62)</f>
+        <f t="shared" si="1"/>
         <v>2013Q1</v>
       </c>
       <c r="D62" s="29">
@@ -8606,7 +8624,7 @@
         <v>12</v>
       </c>
       <c r="C63" s="27" t="str">
-        <f>_xlfn.CONCAT(A63,B63)</f>
+        <f t="shared" si="1"/>
         <v>2013Q2</v>
       </c>
       <c r="D63" s="29">
@@ -8627,7 +8645,7 @@
         <v>13</v>
       </c>
       <c r="C64" s="27" t="str">
-        <f>_xlfn.CONCAT(A64,B64)</f>
+        <f t="shared" si="1"/>
         <v>2013Q3</v>
       </c>
       <c r="D64" s="29">
@@ -8648,7 +8666,7 @@
         <v>14</v>
       </c>
       <c r="C65" s="27" t="str">
-        <f>_xlfn.CONCAT(A65,B65)</f>
+        <f t="shared" si="1"/>
         <v>2013Q4</v>
       </c>
       <c r="D65" s="29">
@@ -8669,7 +8687,7 @@
         <v>15</v>
       </c>
       <c r="C66" s="27" t="str">
-        <f>_xlfn.CONCAT(A66,B66)</f>
+        <f t="shared" si="1"/>
         <v>2014Q1</v>
       </c>
       <c r="D66" s="29">
@@ -8690,7 +8708,7 @@
         <v>12</v>
       </c>
       <c r="C67" s="27" t="str">
-        <f>_xlfn.CONCAT(A67,B67)</f>
+        <f t="shared" si="1"/>
         <v>2014Q2</v>
       </c>
       <c r="D67" s="29">
@@ -8711,7 +8729,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="27" t="str">
-        <f>_xlfn.CONCAT(A68,B68)</f>
+        <f t="shared" ref="C68:C99" si="2">_xlfn.CONCAT(A68,B68)</f>
         <v>2014Q3</v>
       </c>
       <c r="D68" s="29">
@@ -8732,7 +8750,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="27" t="str">
-        <f>_xlfn.CONCAT(A69,B69)</f>
+        <f t="shared" si="2"/>
         <v>2014Q4</v>
       </c>
       <c r="D69" s="29">
@@ -8753,7 +8771,7 @@
         <v>15</v>
       </c>
       <c r="C70" s="27" t="str">
-        <f>_xlfn.CONCAT(A70,B70)</f>
+        <f t="shared" si="2"/>
         <v>2015Q1</v>
       </c>
       <c r="D70" s="29">
@@ -8774,7 +8792,7 @@
         <v>12</v>
       </c>
       <c r="C71" s="27" t="str">
-        <f>_xlfn.CONCAT(A71,B71)</f>
+        <f t="shared" si="2"/>
         <v>2015Q2</v>
       </c>
       <c r="D71" s="29">
@@ -8795,7 +8813,7 @@
         <v>13</v>
       </c>
       <c r="C72" s="27" t="str">
-        <f>_xlfn.CONCAT(A72,B72)</f>
+        <f t="shared" si="2"/>
         <v>2015Q3</v>
       </c>
       <c r="D72" s="29">
@@ -8816,7 +8834,7 @@
         <v>14</v>
       </c>
       <c r="C73" s="27" t="str">
-        <f>_xlfn.CONCAT(A73,B73)</f>
+        <f t="shared" si="2"/>
         <v>2015Q4</v>
       </c>
       <c r="D73" s="29">
@@ -8837,7 +8855,7 @@
         <v>15</v>
       </c>
       <c r="C74" s="27" t="str">
-        <f>_xlfn.CONCAT(A74,B74)</f>
+        <f t="shared" si="2"/>
         <v>2016Q1</v>
       </c>
       <c r="D74" s="29">
@@ -8858,7 +8876,7 @@
         <v>12</v>
       </c>
       <c r="C75" s="27" t="str">
-        <f>_xlfn.CONCAT(A75,B75)</f>
+        <f t="shared" si="2"/>
         <v>2016Q2</v>
       </c>
       <c r="D75" s="29">
@@ -8879,7 +8897,7 @@
         <v>13</v>
       </c>
       <c r="C76" s="27" t="str">
-        <f>_xlfn.CONCAT(A76,B76)</f>
+        <f t="shared" si="2"/>
         <v>2016Q3</v>
       </c>
       <c r="D76" s="29">
@@ -8900,7 +8918,7 @@
         <v>14</v>
       </c>
       <c r="C77" s="27" t="str">
-        <f>_xlfn.CONCAT(A77,B77)</f>
+        <f t="shared" si="2"/>
         <v>2016Q4</v>
       </c>
       <c r="D77" s="29">
@@ -8921,7 +8939,7 @@
         <v>15</v>
       </c>
       <c r="C78" s="27" t="str">
-        <f>_xlfn.CONCAT(A78,B78)</f>
+        <f t="shared" si="2"/>
         <v>2017Q1</v>
       </c>
       <c r="D78" s="29">
@@ -8942,7 +8960,7 @@
         <v>12</v>
       </c>
       <c r="C79" s="27" t="str">
-        <f>_xlfn.CONCAT(A79,B79)</f>
+        <f t="shared" si="2"/>
         <v>2017Q2</v>
       </c>
       <c r="D79" s="29">
@@ -8963,7 +8981,7 @@
         <v>13</v>
       </c>
       <c r="C80" s="27" t="str">
-        <f>_xlfn.CONCAT(A80,B80)</f>
+        <f t="shared" si="2"/>
         <v>2017Q3</v>
       </c>
       <c r="D80" s="29">
@@ -8984,7 +9002,7 @@
         <v>14</v>
       </c>
       <c r="C81" s="27" t="str">
-        <f>_xlfn.CONCAT(A81,B81)</f>
+        <f t="shared" si="2"/>
         <v>2017Q4</v>
       </c>
       <c r="D81" s="29">
@@ -9005,7 +9023,7 @@
         <v>15</v>
       </c>
       <c r="C82" s="27" t="str">
-        <f>_xlfn.CONCAT(A82,B82)</f>
+        <f t="shared" si="2"/>
         <v>2018Q1</v>
       </c>
       <c r="D82" s="29">
@@ -9026,7 +9044,7 @@
         <v>12</v>
       </c>
       <c r="C83" s="27" t="str">
-        <f>_xlfn.CONCAT(A83,B83)</f>
+        <f t="shared" si="2"/>
         <v>2018Q2</v>
       </c>
       <c r="D83" s="29">
@@ -9047,7 +9065,7 @@
         <v>13</v>
       </c>
       <c r="C84" s="27" t="str">
-        <f>_xlfn.CONCAT(A84,B84)</f>
+        <f t="shared" si="2"/>
         <v>2018Q3</v>
       </c>
       <c r="D84" s="29">
@@ -9068,7 +9086,7 @@
         <v>14</v>
       </c>
       <c r="C85" s="27" t="str">
-        <f>_xlfn.CONCAT(A85,B85)</f>
+        <f t="shared" si="2"/>
         <v>2018Q4</v>
       </c>
       <c r="D85" s="29">
@@ -9089,7 +9107,7 @@
         <v>15</v>
       </c>
       <c r="C86" s="27" t="str">
-        <f>_xlfn.CONCAT(A86,B86)</f>
+        <f t="shared" si="2"/>
         <v>2019Q1</v>
       </c>
       <c r="D86" s="29">
@@ -9110,7 +9128,7 @@
         <v>12</v>
       </c>
       <c r="C87" s="27" t="str">
-        <f>_xlfn.CONCAT(A87,B87)</f>
+        <f t="shared" si="2"/>
         <v>2019Q2</v>
       </c>
       <c r="D87" s="29">
@@ -9131,7 +9149,7 @@
         <v>13</v>
       </c>
       <c r="C88" s="27" t="str">
-        <f>_xlfn.CONCAT(A88,B88)</f>
+        <f t="shared" si="2"/>
         <v>2019Q3</v>
       </c>
       <c r="D88" s="29">
@@ -9152,7 +9170,7 @@
         <v>14</v>
       </c>
       <c r="C89" s="27" t="str">
-        <f>_xlfn.CONCAT(A89,B89)</f>
+        <f t="shared" si="2"/>
         <v>2019Q4</v>
       </c>
       <c r="D89" s="29">
@@ -9173,7 +9191,7 @@
         <v>15</v>
       </c>
       <c r="C90" s="27" t="str">
-        <f>_xlfn.CONCAT(A90,B90)</f>
+        <f t="shared" si="2"/>
         <v>2020Q1</v>
       </c>
       <c r="D90" s="29">
@@ -9194,7 +9212,7 @@
         <v>12</v>
       </c>
       <c r="C91" s="27" t="str">
-        <f>_xlfn.CONCAT(A91,B91)</f>
+        <f t="shared" si="2"/>
         <v>2020Q2</v>
       </c>
       <c r="D91" s="29">
@@ -9215,7 +9233,7 @@
         <v>13</v>
       </c>
       <c r="C92" s="27" t="str">
-        <f>_xlfn.CONCAT(A92,B92)</f>
+        <f t="shared" si="2"/>
         <v>2020Q3</v>
       </c>
       <c r="D92" s="29">
@@ -9236,7 +9254,7 @@
         <v>14</v>
       </c>
       <c r="C93" s="27" t="str">
-        <f>_xlfn.CONCAT(A93,B93)</f>
+        <f t="shared" si="2"/>
         <v>2020Q4</v>
       </c>
       <c r="D93" s="29">
@@ -9257,7 +9275,7 @@
         <v>15</v>
       </c>
       <c r="C94" s="27" t="str">
-        <f>_xlfn.CONCAT(A94,B94)</f>
+        <f t="shared" si="2"/>
         <v>2021Q1</v>
       </c>
       <c r="D94" s="29">
@@ -9278,7 +9296,7 @@
         <v>12</v>
       </c>
       <c r="C95" s="27" t="str">
-        <f>_xlfn.CONCAT(A95,B95)</f>
+        <f t="shared" si="2"/>
         <v>2021Q2</v>
       </c>
       <c r="D95" s="29">
@@ -9299,7 +9317,7 @@
         <v>13</v>
       </c>
       <c r="C96" s="27" t="str">
-        <f>_xlfn.CONCAT(A96,B96)</f>
+        <f t="shared" si="2"/>
         <v>2021Q3</v>
       </c>
       <c r="D96" s="29">

</xml_diff>